<commit_message>
adding wolverton 2007 measruement
</commit_message>
<xml_diff>
--- a/terms/masterMapping.xlsx
+++ b/terms/masterMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/terms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36881AE-263F-A04B-8156-B9985D514DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2ED7E9-CE31-D746-8435-9DCAF815A5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16620" xr2:uid="{B955206B-1AD7-A04D-9DC5-27623262407F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="240">
   <si>
     <t>Scott 1985</t>
   </si>
@@ -739,6 +739,12 @@
   </si>
   <si>
     <t>depth of calcaneal body</t>
+  </si>
+  <si>
+    <t>AST4</t>
+  </si>
+  <si>
+    <t>Wolverton 2007</t>
   </si>
 </sst>
 </file>
@@ -1113,11 +1119,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67F0FC0-F849-E045-82AF-DA408F6FE6AB}">
-  <dimension ref="A1:G141"/>
+  <dimension ref="A1:H141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1132,7 @@
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1146,10 +1152,13 @@
         <v>233</v>
       </c>
       <c r="G1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1162,11 +1171,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>188</v>
       </c>
@@ -1176,11 +1185,11 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>189</v>
       </c>
@@ -1190,11 +1199,11 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1207,11 +1216,11 @@
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1221,11 +1230,11 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1238,11 +1247,11 @@
       <c r="D7">
         <v>7</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1253,10 +1262,13 @@
         <v>11</v>
       </c>
       <c r="G8" t="s">
+        <v>238</v>
+      </c>
+      <c r="H8" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1269,11 +1281,11 @@
       <c r="D9">
         <v>5</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>190</v>
       </c>
@@ -1287,7 +1299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1297,11 +1309,11 @@
       <c r="D11">
         <v>4</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1311,11 +1323,11 @@
       <c r="D12">
         <v>6</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1332,7 +1344,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1346,7 +1358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1357,7 +1369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>236</v>
       </c>
@@ -1370,11 +1382,11 @@
       <c r="F16" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>234</v>
       </c>
@@ -1384,11 +1396,11 @@
       <c r="D17">
         <v>4</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>235</v>
       </c>
@@ -1398,11 +1410,11 @@
       <c r="D18">
         <v>5</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1413,7 +1425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>237</v>
       </c>
@@ -1424,7 +1436,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>118</v>
       </c>
@@ -1438,7 +1450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>120</v>
       </c>
@@ -1449,7 +1461,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>122</v>
       </c>
@@ -1462,11 +1474,11 @@
       <c r="D23">
         <v>5</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>125</v>
       </c>
@@ -1476,11 +1488,11 @@
       <c r="C24" t="s">
         <v>123</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>128</v>
       </c>
@@ -1493,11 +1505,11 @@
       <c r="D25">
         <v>10</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>131</v>
       </c>
@@ -1513,11 +1525,11 @@
       <c r="E26" t="s">
         <v>129</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>132</v>
       </c>
@@ -1528,7 +1540,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>134</v>
       </c>
@@ -1541,11 +1553,11 @@
       <c r="D28">
         <v>7</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>135</v>
       </c>
@@ -1562,7 +1574,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>137</v>
       </c>
@@ -1572,11 +1584,11 @@
       <c r="D30">
         <v>6</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>139</v>
       </c>
@@ -1586,11 +1598,11 @@
       <c r="D31">
         <v>8</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>141</v>
       </c>
@@ -1600,11 +1612,11 @@
       <c r="D32">
         <v>9</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>162</v>
       </c>
@@ -1614,11 +1626,11 @@
       <c r="D33">
         <v>4</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>165</v>
       </c>
@@ -1631,11 +1643,11 @@
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>166</v>
       </c>
@@ -1649,7 +1661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>169</v>
       </c>
@@ -1665,11 +1677,11 @@
       <c r="E36" t="s">
         <v>167</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>163</v>
       </c>
@@ -1677,7 +1689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>171</v>
       </c>
@@ -1690,11 +1702,11 @@
       <c r="D38">
         <v>5</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>173</v>
       </c>
@@ -1704,11 +1716,11 @@
       <c r="D39">
         <v>6</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>177</v>
       </c>
@@ -1724,11 +1736,11 @@
       <c r="E40" t="s">
         <v>175</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>179</v>
       </c>
@@ -1738,11 +1750,11 @@
       <c r="D41">
         <v>8</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>180</v>
       </c>
@@ -1753,7 +1765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>181</v>
       </c>
@@ -1764,7 +1776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>182</v>
       </c>
@@ -1775,7 +1787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>183</v>
       </c>
@@ -1786,7 +1798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>185</v>
       </c>
@@ -1796,11 +1808,11 @@
       <c r="C46" t="s">
         <v>102</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>187</v>
       </c>
@@ -1810,11 +1822,11 @@
       <c r="C47" t="s">
         <v>11</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1825,7 +1837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>39</v>
       </c>
@@ -1836,7 +1848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>42</v>
       </c>
@@ -1847,7 +1859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>45</v>
       </c>
@@ -1858,7 +1870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -1869,7 +1881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>85</v>
       </c>
@@ -1880,7 +1892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>34</v>
       </c>
@@ -1891,7 +1903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>41</v>
       </c>
@@ -1902,7 +1914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>46</v>
       </c>
@@ -1916,7 +1928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>64</v>
       </c>
@@ -1929,11 +1941,11 @@
       <c r="D57">
         <v>3</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>77</v>
       </c>
@@ -1946,11 +1958,11 @@
       <c r="D58">
         <v>12</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>81</v>
       </c>
@@ -1961,7 +1973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>82</v>
       </c>
@@ -1972,7 +1984,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>83</v>
       </c>
@@ -1985,11 +1997,11 @@
       <c r="D61">
         <v>5</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>84</v>
       </c>
@@ -2000,7 +2012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>91</v>
       </c>
@@ -2010,9 +2022,9 @@
       <c r="D63" s="2">
         <v>8</v>
       </c>
-      <c r="G63" s="2"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>92</v>
       </c>
@@ -2022,9 +2034,9 @@
       <c r="D64" s="1">
         <v>9</v>
       </c>
-      <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>94</v>
       </c>
@@ -2034,9 +2046,9 @@
       <c r="D65" s="1">
         <v>16</v>
       </c>
-      <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>95</v>
       </c>
@@ -2046,9 +2058,9 @@
       <c r="D66" s="1">
         <v>4</v>
       </c>
-      <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>98</v>
       </c>
@@ -2059,7 +2071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>99</v>
       </c>
@@ -2070,7 +2082,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>38</v>
       </c>
@@ -2081,7 +2093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>40</v>
       </c>
@@ -2092,7 +2104,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>43</v>
       </c>
@@ -2103,7 +2115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>47</v>
       </c>
@@ -2114,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>50</v>
       </c>
@@ -2125,7 +2137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>52</v>
       </c>
@@ -2136,7 +2148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>86</v>
       </c>
@@ -2147,7 +2159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>108</v>
       </c>
@@ -2158,7 +2170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>110</v>
       </c>
@@ -2169,7 +2181,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>112</v>
       </c>
@@ -2180,7 +2192,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>114</v>
       </c>
@@ -2190,11 +2202,11 @@
       <c r="C79" t="s">
         <v>11</v>
       </c>
-      <c r="G79" t="s">
+      <c r="H79" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>116</v>
       </c>
@@ -2205,7 +2217,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>49</v>
       </c>
@@ -2216,7 +2228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>55</v>
       </c>
@@ -2227,7 +2239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>66</v>
       </c>
@@ -2238,7 +2250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>69</v>
       </c>
@@ -2249,7 +2261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>72</v>
       </c>
@@ -2260,7 +2272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>88</v>
       </c>
@@ -2271,7 +2283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>54</v>
       </c>
@@ -2282,7 +2294,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>68</v>
       </c>
@@ -2293,7 +2305,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>79</v>
       </c>
@@ -2304,7 +2316,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>80</v>
       </c>
@@ -2315,7 +2327,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>87</v>
       </c>
@@ -2326,7 +2338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
@@ -2336,9 +2348,9 @@
       <c r="D92" s="1">
         <v>8</v>
       </c>
-      <c r="G92" s="1"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H92" s="1"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>93</v>
       </c>
@@ -2348,9 +2360,9 @@
       <c r="D93" s="1">
         <v>9</v>
       </c>
-      <c r="G93" s="1"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H93" s="1"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>96</v>
       </c>
@@ -2360,9 +2372,9 @@
       <c r="D94" s="1">
         <v>4</v>
       </c>
-      <c r="G94" s="1"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H94" s="1"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>100</v>
       </c>
@@ -2373,7 +2385,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>101</v>
       </c>
@@ -2384,7 +2396,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>61</v>
       </c>
@@ -2397,11 +2409,11 @@
       <c r="D97">
         <v>5</v>
       </c>
-      <c r="G97" t="s">
+      <c r="H97" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>65</v>
       </c>
@@ -2414,11 +2426,11 @@
       <c r="D98">
         <v>3</v>
       </c>
-      <c r="G98" t="s">
+      <c r="H98" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>73</v>
       </c>
@@ -2432,7 +2444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>78</v>
       </c>
@@ -2445,11 +2457,11 @@
       <c r="D100">
         <v>12</v>
       </c>
-      <c r="G100" t="s">
+      <c r="H100" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>104</v>
       </c>
@@ -2459,11 +2471,11 @@
       <c r="C101" t="s">
         <v>102</v>
       </c>
-      <c r="G101" t="s">
+      <c r="H101" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>106</v>
       </c>
@@ -2473,9 +2485,9 @@
       <c r="C102" t="s">
         <v>105</v>
       </c>
-      <c r="G102" s="1"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H102" s="1"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>57</v>
       </c>
@@ -2486,7 +2498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>67</v>
       </c>
@@ -2497,7 +2509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>70</v>
       </c>
@@ -2508,7 +2520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>74</v>
       </c>
@@ -2519,7 +2531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>89</v>
       </c>
@@ -2529,9 +2541,9 @@
       <c r="D107" s="1">
         <v>2</v>
       </c>
-      <c r="G107" s="1"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H107" s="1"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>143</v>
       </c>
@@ -2545,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>144</v>
       </c>
@@ -2556,7 +2568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>146</v>
       </c>
@@ -2569,11 +2581,11 @@
       <c r="D110">
         <v>3</v>
       </c>
-      <c r="G110" t="s">
+      <c r="H110" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>148</v>
       </c>
@@ -2583,11 +2595,11 @@
       <c r="D111">
         <v>4</v>
       </c>
-      <c r="G111" t="s">
+      <c r="H111" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>150</v>
       </c>
@@ -2600,11 +2612,11 @@
       <c r="D112">
         <v>5</v>
       </c>
-      <c r="G112" t="s">
+      <c r="H112" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>152</v>
       </c>
@@ -2614,11 +2626,11 @@
       <c r="D113">
         <v>6</v>
       </c>
-      <c r="G113" t="s">
+      <c r="H113" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>154</v>
       </c>
@@ -2631,11 +2643,11 @@
       <c r="D114">
         <v>7</v>
       </c>
-      <c r="G114" t="s">
+      <c r="H114" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>156</v>
       </c>
@@ -2648,11 +2660,11 @@
       <c r="D115">
         <v>8</v>
       </c>
-      <c r="G115" t="s">
+      <c r="H115" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>202</v>
       </c>
@@ -2662,11 +2674,11 @@
       <c r="D116">
         <v>9</v>
       </c>
-      <c r="G116" s="3" t="s">
+      <c r="H116" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>158</v>
       </c>
@@ -2677,7 +2689,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>159</v>
       </c>
@@ -2688,18 +2700,18 @@
         <v>109</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B119" s="2"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>203</v>
       </c>
@@ -2713,7 +2725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>204</v>
       </c>
@@ -2727,7 +2739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>212</v>
       </c>
@@ -2741,7 +2753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>207</v>
       </c>
@@ -2755,7 +2767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>209</v>
       </c>
@@ -2769,7 +2781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>213</v>
       </c>
@@ -2777,7 +2789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>214</v>
       </c>
@@ -2791,7 +2803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>215</v>
       </c>

</xml_diff>